<commit_message>
bringing in old blogposts
</commit_message>
<xml_diff>
--- a/scrap/events.xlsx
+++ b/scrap/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charliejhadley/Github/visibledata.github.io/scrap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41771DCC-7FF4-104D-B6D3-A6D20473C085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4FFE38-916D-4E47-90A1-123152B5A3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="500" windowWidth="25280" windowHeight="28300" xr2:uid="{F73A2A0E-E40C-2440-A145-0DD172556E49}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Year</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Visiting Lectureship</t>
+  </si>
+  <si>
+    <t>American University in Cairo</t>
   </si>
 </sst>
 </file>
@@ -519,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C7B049-68D6-454E-9AF5-0049DAB5CA47}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,6 +770,9 @@
       <c r="C13" t="s">
         <v>39</v>
       </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
update with new blogpost
</commit_message>
<xml_diff>
--- a/scrap/events.xlsx
+++ b/scrap/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charliejhadley/Github/visibledata.github.io/scrap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4FFE38-916D-4E47-90A1-123152B5A3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDD3283-2E8D-6E4D-B2F2-1AE4BB2C8F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="500" windowWidth="25280" windowHeight="28300" xr2:uid="{F73A2A0E-E40C-2440-A145-0DD172556E49}"/>
+    <workbookView xWindow="25920" yWindow="500" windowWidth="25280" windowHeight="28300" xr2:uid="{F73A2A0E-E40C-2440-A145-0DD172556E49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Year</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>https://www.rladieschicago.org/talk/2019-12-4-meetup/</t>
-  </si>
-  <si>
     <t>Workshop</t>
   </si>
   <si>
@@ -158,6 +155,12 @@
   </si>
   <si>
     <t>American University in Cairo</t>
+  </si>
+  <si>
+    <t>Using interactive data visualisations to tell stories</t>
+  </si>
+  <si>
+    <t>Royal Statistical Society Conference</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C7B049-68D6-454E-9AF5-0049DAB5CA47}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -546,13 +549,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
         <v>11</v>
@@ -569,7 +572,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -583,13 +586,13 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -600,13 +603,13 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -617,16 +620,16 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -640,10 +643,10 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -651,19 +654,19 @@
         <v>2018</v>
       </c>
       <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -671,16 +674,16 @@
         <v>2017</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -688,19 +691,19 @@
         <v>2017</v>
       </c>
       <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
         <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -711,53 +714,51 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2016</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>24</v>
@@ -765,21 +766,41 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>2016</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>2014</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
         <v>39</v>
-      </c>
-      <c r="D13" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G10" r:id="rId1" xr:uid="{8C33AC0A-FA96-5647-B0C8-0B4BF1CC78ED}"/>
     <hyperlink ref="G7" r:id="rId2" xr:uid="{051C4584-E859-754D-A4E3-7A10345839BC}"/>
-    <hyperlink ref="G12" r:id="rId3" xr:uid="{60D6093F-75C9-B04C-A3E1-5028038D4443}"/>
-    <hyperlink ref="G11" r:id="rId4" xr:uid="{D1F72734-E4A1-5148-AB1A-C0CBA7769426}"/>
+    <hyperlink ref="G13" r:id="rId3" xr:uid="{60D6093F-75C9-B04C-A3E1-5028038D4443}"/>
+    <hyperlink ref="G12" r:id="rId4" xr:uid="{D1F72734-E4A1-5148-AB1A-C0CBA7769426}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>